<commit_message>
Added 6 Countries to Excel and Added .env example file
</commit_message>
<xml_diff>
--- a/backend/data/country_data.xlsx
+++ b/backend/data/country_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AI-Country-Risk-Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AiCountryRisk\backend-dev\AI-Country-Risk-Dashboard\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD962CF2-214A-4CE8-95B6-B0407B057C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C262F0F5-1D58-488D-AEEC-8A99AA241AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>iso2Code</t>
   </si>
@@ -504,6 +504,60 @@
   </si>
   <si>
     <t>Corruption Index (2024)</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>TUR</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>RUS</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>MNG</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>KAZ</t>
+  </si>
+  <si>
+    <t>KZ</t>
   </si>
 </sst>
 </file>
@@ -511,7 +565,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -576,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -881,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,82 +973,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5">
-        <v>-58.417299999999997</v>
+        <v>54.3705</v>
       </c>
       <c r="F2" s="5">
-        <v>-34.611800000000002</v>
+        <v>24.476400000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E3" s="5">
-        <v>149.12899999999999</v>
+        <v>-58.417299999999997</v>
       </c>
       <c r="F3" s="5">
-        <v>-35.281999999999996</v>
+        <v>-34.611800000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E4" s="5">
-        <v>16.379799999999999</v>
+        <v>149.12899999999999</v>
       </c>
       <c r="F4" s="5">
-        <v>48.220100000000002</v>
+        <v>-35.281999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="E5" s="5">
-        <v>90.411299999999997</v>
+        <v>16.379799999999999</v>
       </c>
       <c r="F5" s="5">
-        <v>23.705500000000001</v>
+        <v>48.220100000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,902 +1073,1022 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
         <v>23</v>
       </c>
-      <c r="D7" s="4">
-        <v>34</v>
-      </c>
       <c r="E7" s="5">
-        <v>-47.929200000000002</v>
+        <v>90.411299999999997</v>
       </c>
       <c r="F7" s="5">
-        <v>-15.780099999999999</v>
+        <v>23.705500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5">
-        <v>-75.691900000000004</v>
+        <v>-47.929200000000002</v>
       </c>
       <c r="F8" s="5">
-        <v>45.421500000000002</v>
+        <v>-15.780099999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E9" s="5">
-        <v>-70.647499999999994</v>
+        <v>-75.691900000000004</v>
       </c>
       <c r="F9" s="5">
-        <v>-33.475000000000001</v>
+        <v>45.421500000000002</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="E10" s="5">
-        <v>116.286</v>
+        <v>7.4482100000000004</v>
       </c>
       <c r="F10" s="5">
-        <v>40.049500000000002</v>
+        <v>46.948</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="E11" s="5">
-        <v>-74.081999999999994</v>
+        <v>-70.647499999999994</v>
       </c>
       <c r="F11" s="5">
-        <v>4.6098699999999999</v>
+        <v>-33.475000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4">
         <v>43</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="4">
-        <v>90</v>
-      </c>
       <c r="E12" s="5">
-        <v>12.568099999999999</v>
+        <v>116.286</v>
       </c>
       <c r="F12" s="5">
-        <v>55.676299999999998</v>
+        <v>40.049500000000002</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5">
-        <v>24.952500000000001</v>
+        <v>-74.081999999999994</v>
       </c>
       <c r="F13" s="5">
-        <v>60.160800000000002</v>
+        <v>4.6098699999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E14" s="5">
-        <v>2.3509699999999998</v>
+        <v>13.4115</v>
       </c>
       <c r="F14" s="5">
-        <v>48.8566</v>
+        <v>52.523499999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E15" s="5">
-        <v>13.4115</v>
+        <v>12.568099999999999</v>
       </c>
       <c r="F15" s="5">
-        <v>52.523499999999999</v>
+        <v>55.676299999999998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5">
-        <v>23.7166</v>
+        <v>-3.7032699999999998</v>
       </c>
       <c r="F16" s="5">
-        <v>37.979199999999999</v>
+        <v>40.416699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E17" s="5">
-        <v>114.10899999999999</v>
+        <v>24.952500000000001</v>
       </c>
       <c r="F17" s="5">
-        <v>22.3964</v>
+        <v>60.160800000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E18" s="5">
-        <v>19.040800000000001</v>
+        <v>2.3509699999999998</v>
       </c>
       <c r="F18" s="5">
-        <v>47.498399999999997</v>
+        <v>48.8566</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="4">
         <v>71</v>
       </c>
-      <c r="D19" s="4">
-        <v>38</v>
-      </c>
       <c r="E19" s="5">
-        <v>77.224999999999994</v>
+        <v>-0.12623599999999999</v>
       </c>
       <c r="F19" s="5">
-        <v>28.635300000000001</v>
+        <v>51.5002</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D20" s="4">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E20" s="5">
-        <v>106.83</v>
+        <v>23.7166</v>
       </c>
       <c r="F20" s="5">
-        <v>-6.1975199999999999</v>
+        <v>37.979199999999999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="4">
         <v>74</v>
       </c>
-      <c r="D21" s="4">
-        <v>77</v>
-      </c>
       <c r="E21" s="5">
-        <v>-6.2674899999999996</v>
+        <v>114.10899999999999</v>
       </c>
       <c r="F21" s="5">
-        <v>53.344099999999997</v>
+        <v>22.3964</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D22" s="4">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E22" s="5">
-        <v>35.203499999999998</v>
+        <v>19.040800000000001</v>
       </c>
       <c r="F22" s="5">
-        <v>31.771699999999999</v>
+        <v>47.498399999999997</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D23" s="4">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E23" s="5">
-        <v>12.4823</v>
+        <v>106.83</v>
       </c>
       <c r="F23" s="5">
-        <v>41.895499999999998</v>
+        <v>-6.1975199999999999</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D24" s="4">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E24" s="5">
-        <v>139.77000000000001</v>
+        <v>77.224999999999994</v>
       </c>
       <c r="F24" s="5">
-        <v>35.67</v>
+        <v>28.635300000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D25" s="4">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E25" s="5">
-        <v>36.812600000000003</v>
+        <v>-6.2674899999999996</v>
       </c>
       <c r="F25" s="5">
-        <v>-1.2797499999999999</v>
+        <v>53.344099999999997</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D26" s="4">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E26" s="5">
-        <v>6.1295999999999999</v>
+        <v>35.203499999999998</v>
       </c>
       <c r="F26" s="5">
-        <v>49.61</v>
+        <v>31.771699999999999</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D27" s="4">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E27" s="5">
-        <v>101.684</v>
+        <v>12.4823</v>
       </c>
       <c r="F27" s="5">
-        <v>3.1243300000000001</v>
+        <v>41.895499999999998</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D28" s="4">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E28" s="5">
-        <v>-99.127600000000001</v>
+        <v>139.77000000000001</v>
       </c>
       <c r="F28" s="5">
-        <v>19.427</v>
+        <v>35.67</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>90</v>
+        <v>172</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="D29" s="4">
-        <v>37</v>
-      </c>
-      <c r="E29" s="5">
-        <v>-6.8704000000000001</v>
-      </c>
-      <c r="F29" s="5">
-        <v>33.990499999999997</v>
+        <v>88</v>
+      </c>
+      <c r="E29" s="4">
+        <v>71.449100000000001</v>
+      </c>
+      <c r="F29" s="4">
+        <v>51.169400000000003</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D30" s="4">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="E30" s="5">
-        <v>4.8909500000000001</v>
+        <v>36.812600000000003</v>
       </c>
       <c r="F30" s="5">
-        <v>52.373800000000003</v>
+        <v>-1.2797499999999999</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="D31" s="4">
-        <v>83</v>
-      </c>
-      <c r="E31" s="5">
-        <v>174.77600000000001</v>
-      </c>
-      <c r="F31" s="5">
-        <v>-41.286499999999997</v>
+        <v>30</v>
+      </c>
+      <c r="E31" s="4">
+        <v>126.97799999999999</v>
+      </c>
+      <c r="F31" s="4">
+        <v>37.566499999999998</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D32" s="4">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="E32" s="5">
-        <v>7.4890600000000003</v>
+        <v>6.1295999999999999</v>
       </c>
       <c r="F32" s="5">
-        <v>9.0580400000000001</v>
+        <v>49.61</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="D33" s="4">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E33" s="5">
-        <v>10.7387</v>
+        <v>-6.8704000000000001</v>
       </c>
       <c r="F33" s="5">
-        <v>59.913800000000002</v>
+        <v>33.990499999999997</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D34" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="5">
-        <v>72.8</v>
+        <v>-99.127600000000001</v>
       </c>
       <c r="F34" s="5">
-        <v>30.5167</v>
+        <v>19.427</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="4">
         <v>114</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="4">
-        <v>31</v>
-      </c>
-      <c r="E35" s="5">
-        <v>-77.046499999999995</v>
-      </c>
-      <c r="F35" s="5">
-        <v>-12.0931</v>
+      <c r="E35" s="4">
+        <v>106.9057</v>
+      </c>
+      <c r="F35" s="4">
+        <v>47.886400000000002</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D36" s="4">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5">
-        <v>121.035</v>
+        <v>101.684</v>
       </c>
       <c r="F36" s="5">
-        <v>14.551500000000001</v>
+        <v>3.1243300000000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D37" s="4">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E37" s="5">
-        <v>21.02</v>
+        <v>7.4890600000000003</v>
       </c>
       <c r="F37" s="5">
-        <v>52.26</v>
+        <v>9.0580400000000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D38" s="4">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E38" s="5">
-        <v>-9.1355199999999996</v>
+        <v>4.8909500000000001</v>
       </c>
       <c r="F38" s="5">
-        <v>38.7072</v>
+        <v>52.373800000000003</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D39" s="4">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E39" s="5">
-        <v>51.508200000000002</v>
+        <v>10.7387</v>
       </c>
       <c r="F39" s="5">
-        <v>25.294799999999999</v>
+        <v>59.913800000000002</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D40" s="4">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="E40" s="5">
-        <v>26.097899999999999</v>
+        <v>174.77600000000001</v>
       </c>
       <c r="F40" s="5">
-        <v>44.447899999999997</v>
+        <v>-41.286499999999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D41" s="4">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E41" s="5">
-        <v>46.697699999999998</v>
+        <v>72.8</v>
       </c>
       <c r="F41" s="5">
-        <v>24.674800000000001</v>
+        <v>30.5167</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="D42" s="4">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="E42" s="5">
-        <v>103.85</v>
+        <v>-77.046499999999995</v>
       </c>
       <c r="F42" s="5">
-        <v>1.2894099999999999</v>
+        <v>-12.0931</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="D43" s="4">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E43" s="5">
-        <v>28.187100000000001</v>
+        <v>121.035</v>
       </c>
       <c r="F43" s="5">
-        <v>-25.745999999999999</v>
+        <v>14.551500000000001</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="D44" s="4">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E44" s="5">
-        <v>-3.7032699999999998</v>
+        <v>21.02</v>
       </c>
       <c r="F44" s="5">
-        <v>40.416699999999999</v>
+        <v>52.26</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D45" s="4">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E45" s="5">
-        <v>18.064499999999999</v>
+        <v>-9.1355199999999996</v>
       </c>
       <c r="F45" s="5">
-        <v>59.332700000000003</v>
+        <v>38.7072</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="D46" s="4">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E46" s="5">
-        <v>7.4482100000000004</v>
+        <v>51.508200000000002</v>
       </c>
       <c r="F46" s="5">
-        <v>46.948</v>
+        <v>25.294799999999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D47" s="4">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E47" s="5">
-        <v>100.521</v>
+        <v>26.097899999999999</v>
       </c>
       <c r="F47" s="5">
-        <v>13.7308</v>
+        <v>44.447899999999997</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="D48" s="4">
-        <v>35</v>
-      </c>
-      <c r="E48" s="5">
-        <v>30.503799999999998</v>
-      </c>
-      <c r="F48" s="5">
-        <v>50.453600000000002</v>
+        <v>154</v>
+      </c>
+      <c r="E48" s="4">
+        <v>37.6173</v>
+      </c>
+      <c r="F48" s="4">
+        <v>55.755800000000001</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="D49" s="4">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E49" s="5">
-        <v>54.3705</v>
+        <v>46.697699999999998</v>
       </c>
       <c r="F49" s="5">
-        <v>24.476400000000002</v>
+        <v>24.674800000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="D50" s="4">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E50" s="5">
-        <v>-0.12623599999999999</v>
+        <v>103.85</v>
       </c>
       <c r="F50" s="5">
-        <v>51.5002</v>
+        <v>1.2894099999999999</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="4">
+        <v>80</v>
+      </c>
+      <c r="E51" s="5">
+        <v>18.064499999999999</v>
+      </c>
+      <c r="F51" s="5">
+        <v>59.332700000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="4">
+        <v>34</v>
+      </c>
+      <c r="E52" s="5">
+        <v>100.521</v>
+      </c>
+      <c r="F52" s="5">
+        <v>13.7308</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="4">
+        <v>107</v>
+      </c>
+      <c r="E53" s="4">
+        <v>32.859699999999997</v>
+      </c>
+      <c r="F53" s="4">
+        <v>39.933399999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="4">
+        <v>25</v>
+      </c>
+      <c r="E54" s="4">
+        <v>121.5654</v>
+      </c>
+      <c r="F54" s="4">
+        <v>25.033000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="4">
+        <v>35</v>
+      </c>
+      <c r="E55" s="5">
+        <v>30.503799999999998</v>
+      </c>
+      <c r="F55" s="5">
+        <v>50.453600000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D56" s="4">
         <v>65</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E56" s="5">
         <v>-77.031999999999996</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F56" s="5">
         <v>38.889499999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="4">
+        <v>41</v>
+      </c>
+      <c r="E57" s="5">
+        <v>28.187100000000001</v>
+      </c>
+      <c r="F57" s="5">
+        <v>-25.745999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved World Bank Data Fetch: Checks for Missing Countries and Runs Them & Handles Countries That's Missing All Data
</commit_message>
<xml_diff>
--- a/backend/data/country_data.xlsx
+++ b/backend/data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AiCountryRisk\backend-dev\AI-Country-Risk-Dashboard\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C262F0F5-1D58-488D-AEEC-8A99AA241AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEFC934-2EAF-4802-9914-F886C22357A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1522,7 @@
         <v>173</v>
       </c>
       <c r="D29" s="4">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="E29" s="4">
         <v>71.449100000000001</v>
@@ -1562,7 +1562,7 @@
         <v>165</v>
       </c>
       <c r="D31" s="4">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="E31" s="4">
         <v>126.97799999999999</v>
@@ -1642,7 +1642,7 @@
         <v>171</v>
       </c>
       <c r="D35" s="4">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="E35" s="4">
         <v>106.9057</v>
@@ -1902,7 +1902,7 @@
         <v>169</v>
       </c>
       <c r="D48" s="4">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="E48" s="4">
         <v>37.6173</v>
@@ -2002,7 +2002,7 @@
         <v>167</v>
       </c>
       <c r="D53" s="4">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="E53" s="4">
         <v>32.859699999999997</v>
@@ -2022,7 +2022,7 @@
         <v>163</v>
       </c>
       <c r="D54" s="4">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E54" s="4">
         <v>121.5654</v>

</xml_diff>

<commit_message>
Removed Taiwan from List of Countries Due to Lack of Data from the World Bank
</commit_message>
<xml_diff>
--- a/backend/data/country_data.xlsx
+++ b/backend/data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AiCountryRisk\backend-dev\AI-Country-Risk-Dashboard\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEFC934-2EAF-4802-9914-F886C22357A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE729C74-3770-4E72-89DC-74FB7C594BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6450" yWindow="2310" windowWidth="17760" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
   <si>
     <t>iso2Code</t>
   </si>
@@ -506,9 +506,6 @@
     <t>Corruption Index (2024)</t>
   </si>
   <si>
-    <t>Taiwan</t>
-  </si>
-  <si>
     <t>South Korea</t>
   </si>
   <si>
@@ -522,12 +519,6 @@
   </si>
   <si>
     <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>TWN</t>
-  </si>
-  <si>
-    <t>TW</t>
   </si>
   <si>
     <t>KOR</t>
@@ -935,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,13 +1504,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D29" s="4">
         <v>40</v>
@@ -1553,13 +1544,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D31" s="4">
         <v>64</v>
@@ -1633,13 +1624,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D35" s="4">
         <v>33</v>
@@ -1893,13 +1884,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D48" s="4">
         <v>22</v>
@@ -1993,13 +1984,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D53" s="4">
         <v>34</v>
@@ -2013,81 +2004,61 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D54" s="4">
-        <v>67</v>
-      </c>
-      <c r="E54" s="4">
-        <v>121.5654</v>
-      </c>
-      <c r="F54" s="4">
-        <v>25.033000000000001</v>
+        <v>35</v>
+      </c>
+      <c r="E54" s="5">
+        <v>30.503799999999998</v>
+      </c>
+      <c r="F54" s="5">
+        <v>50.453600000000002</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D55" s="4">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E55" s="5">
-        <v>30.503799999999998</v>
+        <v>-77.031999999999996</v>
       </c>
       <c r="F55" s="5">
-        <v>50.453600000000002</v>
+        <v>38.889499999999998</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D56" s="4">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E56" s="5">
-        <v>-77.031999999999996</v>
+        <v>28.187100000000001</v>
       </c>
       <c r="F56" s="5">
-        <v>38.889499999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="4">
-        <v>41</v>
-      </c>
-      <c r="E57" s="5">
-        <v>28.187100000000001</v>
-      </c>
-      <c r="F57" s="5">
         <v>-25.745999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Venezuela to country list
</commit_message>
<xml_diff>
--- a/backend/data/country_data.xlsx
+++ b/backend/data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AiCountryRisk\backend-dev\AI-Country-Risk-Dashboard\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE729C74-3770-4E72-89DC-74FB7C594BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD92D4E-F9A4-4E09-B007-4F121E880723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="2310" windowWidth="17760" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="2655" windowWidth="17760" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>iso2Code</t>
   </si>
@@ -549,6 +549,15 @@
   </si>
   <si>
     <t>KZ</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>VE</t>
   </si>
 </sst>
 </file>
@@ -926,11 +935,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2044,21 +2051,41 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="4">
+        <v>10</v>
+      </c>
+      <c r="E56" s="4">
+        <v>-66.903599999999997</v>
+      </c>
+      <c r="F56" s="4">
+        <v>10.480600000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <v>41</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E57" s="5">
         <v>28.187100000000001</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F57" s="5">
         <v>-25.745999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Egypt to List of Countries
</commit_message>
<xml_diff>
--- a/backend/data/country_data.xlsx
+++ b/backend/data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\linux\Projects\AiCountryRisk\backend-dev\AI-Country-Risk-Dashboard\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD92D4E-F9A4-4E09-B007-4F121E880723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E2D40A-FA5E-47AB-A164-AEA52135377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="2655" windowWidth="17760" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="1635" windowWidth="17760" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t>iso2Code</t>
   </si>
@@ -558,6 +558,15 @@
   </si>
   <si>
     <t>VE</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>EGY</t>
+  </si>
+  <si>
+    <t>EG</t>
   </si>
 </sst>
 </file>
@@ -935,9 +944,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,841 +1262,861 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>174</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="D16" s="4">
-        <v>56</v>
-      </c>
-      <c r="E16" s="5">
-        <v>-3.7032699999999998</v>
-      </c>
-      <c r="F16" s="5">
-        <v>40.416699999999999</v>
+        <v>30</v>
+      </c>
+      <c r="E16" s="4">
+        <v>31.235700000000001</v>
+      </c>
+      <c r="F16" s="4">
+        <v>30.0444</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E17" s="5">
-        <v>24.952500000000001</v>
+        <v>-3.7032699999999998</v>
       </c>
       <c r="F17" s="5">
-        <v>60.160800000000002</v>
+        <v>40.416699999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E18" s="5">
-        <v>2.3509699999999998</v>
+        <v>24.952500000000001</v>
       </c>
       <c r="F18" s="5">
-        <v>48.8566</v>
+        <v>60.160800000000002</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E19" s="5">
-        <v>-0.12623599999999999</v>
+        <v>2.3509699999999998</v>
       </c>
       <c r="F19" s="5">
-        <v>51.5002</v>
+        <v>48.8566</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E20" s="5">
-        <v>23.7166</v>
+        <v>-0.12623599999999999</v>
       </c>
       <c r="F20" s="5">
-        <v>37.979199999999999</v>
+        <v>51.5002</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" s="4">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E21" s="5">
-        <v>114.10899999999999</v>
+        <v>23.7166</v>
       </c>
       <c r="F21" s="5">
-        <v>22.3964</v>
+        <v>37.979199999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D22" s="4">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="E22" s="5">
-        <v>19.040800000000001</v>
+        <v>114.10899999999999</v>
       </c>
       <c r="F22" s="5">
-        <v>47.498399999999997</v>
+        <v>22.3964</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D23" s="4">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E23" s="5">
-        <v>106.83</v>
+        <v>19.040800000000001</v>
       </c>
       <c r="F23" s="5">
-        <v>-6.1975199999999999</v>
+        <v>47.498399999999997</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D24" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="5">
-        <v>77.224999999999994</v>
+        <v>106.83</v>
       </c>
       <c r="F24" s="5">
-        <v>28.635300000000001</v>
+        <v>-6.1975199999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D25" s="4">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E25" s="5">
-        <v>-6.2674899999999996</v>
+        <v>77.224999999999994</v>
       </c>
       <c r="F25" s="5">
-        <v>53.344099999999997</v>
+        <v>28.635300000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="4">
         <v>77</v>
       </c>
-      <c r="D26" s="4">
-        <v>64</v>
-      </c>
       <c r="E26" s="5">
-        <v>35.203499999999998</v>
+        <v>-6.2674899999999996</v>
       </c>
       <c r="F26" s="5">
-        <v>31.771699999999999</v>
+        <v>53.344099999999997</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D27" s="4">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E27" s="5">
-        <v>12.4823</v>
+        <v>35.203499999999998</v>
       </c>
       <c r="F27" s="5">
-        <v>41.895499999999998</v>
+        <v>31.771699999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D28" s="4">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E28" s="5">
-        <v>139.77000000000001</v>
+        <v>12.4823</v>
       </c>
       <c r="F28" s="5">
-        <v>35.67</v>
+        <v>41.895499999999998</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>170</v>
+        <v>83</v>
       </c>
       <c r="D29" s="4">
-        <v>40</v>
-      </c>
-      <c r="E29" s="4">
-        <v>71.449100000000001</v>
-      </c>
-      <c r="F29" s="4">
-        <v>51.169400000000003</v>
+        <v>71</v>
+      </c>
+      <c r="E29" s="5">
+        <v>139.77000000000001</v>
+      </c>
+      <c r="F29" s="5">
+        <v>35.67</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="D30" s="4">
-        <v>32</v>
-      </c>
-      <c r="E30" s="5">
-        <v>36.812600000000003</v>
-      </c>
-      <c r="F30" s="5">
-        <v>-1.2797499999999999</v>
+        <v>40</v>
+      </c>
+      <c r="E30" s="4">
+        <v>71.449100000000001</v>
+      </c>
+      <c r="F30" s="4">
+        <v>51.169400000000003</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="D31" s="4">
-        <v>64</v>
-      </c>
-      <c r="E31" s="4">
-        <v>126.97799999999999</v>
-      </c>
-      <c r="F31" s="4">
-        <v>37.566499999999998</v>
+        <v>32</v>
+      </c>
+      <c r="E31" s="5">
+        <v>36.812600000000003</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-1.2797499999999999</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="D32" s="4">
-        <v>81</v>
-      </c>
-      <c r="E32" s="5">
-        <v>6.1295999999999999</v>
-      </c>
-      <c r="F32" s="5">
-        <v>49.61</v>
+        <v>64</v>
+      </c>
+      <c r="E32" s="4">
+        <v>126.97799999999999</v>
+      </c>
+      <c r="F32" s="4">
+        <v>37.566499999999998</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D33" s="4">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="E33" s="5">
-        <v>-6.8704000000000001</v>
+        <v>6.1295999999999999</v>
       </c>
       <c r="F33" s="5">
-        <v>33.990499999999997</v>
+        <v>49.61</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="4">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E34" s="5">
-        <v>-99.127600000000001</v>
+        <v>-6.8704000000000001</v>
       </c>
       <c r="F34" s="5">
-        <v>19.427</v>
+        <v>33.990499999999997</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="D35" s="4">
-        <v>33</v>
-      </c>
-      <c r="E35" s="4">
-        <v>106.9057</v>
-      </c>
-      <c r="F35" s="4">
-        <v>47.886400000000002</v>
+        <v>26</v>
+      </c>
+      <c r="E35" s="5">
+        <v>-99.127600000000001</v>
+      </c>
+      <c r="F35" s="5">
+        <v>19.427</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="D36" s="4">
-        <v>50</v>
-      </c>
-      <c r="E36" s="5">
-        <v>101.684</v>
-      </c>
-      <c r="F36" s="5">
-        <v>3.1243300000000001</v>
+        <v>33</v>
+      </c>
+      <c r="E36" s="4">
+        <v>106.9057</v>
+      </c>
+      <c r="F36" s="4">
+        <v>47.886400000000002</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D37" s="4">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E37" s="5">
-        <v>7.4890600000000003</v>
+        <v>101.684</v>
       </c>
       <c r="F37" s="5">
-        <v>9.0580400000000001</v>
+        <v>3.1243300000000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D38" s="4">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E38" s="5">
-        <v>4.8909500000000001</v>
+        <v>7.4890600000000003</v>
       </c>
       <c r="F38" s="5">
-        <v>52.373800000000003</v>
+        <v>9.0580400000000001</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D39" s="4">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E39" s="5">
-        <v>10.7387</v>
+        <v>4.8909500000000001</v>
       </c>
       <c r="F39" s="5">
-        <v>59.913800000000002</v>
+        <v>52.373800000000003</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D40" s="4">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E40" s="5">
-        <v>174.77600000000001</v>
+        <v>10.7387</v>
       </c>
       <c r="F40" s="5">
-        <v>-41.286499999999997</v>
+        <v>59.913800000000002</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D41" s="4">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="E41" s="5">
-        <v>72.8</v>
+        <v>174.77600000000001</v>
       </c>
       <c r="F41" s="5">
-        <v>30.5167</v>
+        <v>-41.286499999999997</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D42" s="4">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E42" s="5">
-        <v>-77.046499999999995</v>
+        <v>72.8</v>
       </c>
       <c r="F42" s="5">
-        <v>-12.0931</v>
+        <v>30.5167</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D43" s="4">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E43" s="5">
-        <v>121.035</v>
+        <v>-77.046499999999995</v>
       </c>
       <c r="F43" s="5">
-        <v>14.551500000000001</v>
+        <v>-12.0931</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D44" s="4">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E44" s="5">
-        <v>21.02</v>
+        <v>121.035</v>
       </c>
       <c r="F44" s="5">
-        <v>52.26</v>
+        <v>14.551500000000001</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D45" s="4">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E45" s="5">
-        <v>-9.1355199999999996</v>
+        <v>21.02</v>
       </c>
       <c r="F45" s="5">
-        <v>38.7072</v>
+        <v>52.26</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D46" s="4">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E46" s="5">
-        <v>51.508200000000002</v>
+        <v>-9.1355199999999996</v>
       </c>
       <c r="F46" s="5">
-        <v>25.294799999999999</v>
+        <v>38.7072</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D47" s="4">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E47" s="5">
-        <v>26.097899999999999</v>
+        <v>51.508200000000002</v>
       </c>
       <c r="F47" s="5">
-        <v>44.447899999999997</v>
+        <v>25.294799999999999</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="D48" s="4">
-        <v>22</v>
-      </c>
-      <c r="E48" s="4">
-        <v>37.6173</v>
-      </c>
-      <c r="F48" s="4">
-        <v>55.755800000000001</v>
+        <v>46</v>
+      </c>
+      <c r="E48" s="5">
+        <v>26.097899999999999</v>
+      </c>
+      <c r="F48" s="5">
+        <v>44.447899999999997</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="D49" s="4">
-        <v>59</v>
-      </c>
-      <c r="E49" s="5">
-        <v>46.697699999999998</v>
-      </c>
-      <c r="F49" s="5">
-        <v>24.674800000000001</v>
+        <v>22</v>
+      </c>
+      <c r="E49" s="4">
+        <v>37.6173</v>
+      </c>
+      <c r="F49" s="4">
+        <v>55.755800000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D50" s="4">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E50" s="5">
-        <v>103.85</v>
+        <v>46.697699999999998</v>
       </c>
       <c r="F50" s="5">
-        <v>1.2894099999999999</v>
+        <v>24.674800000000001</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D51" s="4">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E51" s="5">
-        <v>18.064499999999999</v>
+        <v>103.85</v>
       </c>
       <c r="F51" s="5">
-        <v>59.332700000000003</v>
+        <v>1.2894099999999999</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D52" s="4">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="E52" s="5">
-        <v>100.521</v>
+        <v>18.064499999999999</v>
       </c>
       <c r="F52" s="5">
-        <v>13.7308</v>
+        <v>59.332700000000003</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="D53" s="4">
         <v>34</v>
       </c>
-      <c r="E53" s="4">
-        <v>32.859699999999997</v>
-      </c>
-      <c r="F53" s="4">
-        <v>39.933399999999999</v>
+      <c r="E53" s="5">
+        <v>100.521</v>
+      </c>
+      <c r="F53" s="5">
+        <v>13.7308</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="D54" s="4">
-        <v>35</v>
-      </c>
-      <c r="E54" s="5">
-        <v>30.503799999999998</v>
-      </c>
-      <c r="F54" s="5">
-        <v>50.453600000000002</v>
+        <v>34</v>
+      </c>
+      <c r="E54" s="4">
+        <v>32.859699999999997</v>
+      </c>
+      <c r="F54" s="4">
+        <v>39.933399999999999</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D55" s="4">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E55" s="5">
-        <v>-77.031999999999996</v>
+        <v>30.503799999999998</v>
       </c>
       <c r="F55" s="5">
-        <v>38.889499999999998</v>
+        <v>50.453600000000002</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D56" s="4">
-        <v>10</v>
-      </c>
-      <c r="E56" s="4">
-        <v>-66.903599999999997</v>
-      </c>
-      <c r="F56" s="4">
-        <v>10.480600000000001</v>
+        <v>65</v>
+      </c>
+      <c r="E56" s="5">
+        <v>-77.031999999999996</v>
+      </c>
+      <c r="F56" s="5">
+        <v>38.889499999999998</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D57" s="4">
+        <v>10</v>
+      </c>
+      <c r="E57" s="4">
+        <v>-66.903599999999997</v>
+      </c>
+      <c r="F57" s="4">
+        <v>10.480600000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <v>41</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E58" s="5">
         <v>28.187100000000001</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F58" s="5">
         <v>-25.745999999999999</v>
       </c>
     </row>

</xml_diff>